<commit_message>
Valkyrie Mech (Continued) 업데이트
#1160
</commit_message>
<xml_diff>
--- a/Data/Zaljerem/Valkyrie Mech (Continued) - 3171145240/3171145240.xlsx
+++ b/Data/Zaljerem/Valkyrie Mech (Continued) - 3171145240/3171145240.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.3\Valkyrie Mech (Continued) - 3171145240\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.9.1\Valkyrie Mech (Continued) - 3171145240\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF84FD6C-A1F6-4B74-B3D9-393A4B86C7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CF690B-3696-4C39-BB8D-4B03DD94728C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="38380" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Main_240502" sheetId="1" r:id="rId1"/>
+    <sheet name="Main_240714" sheetId="1" r:id="rId1"/>
+    <sheet name="Old_240502" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="137">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -74,226 +75,321 @@
     <t>ranged valkyrie</t>
   </si>
   <si>
+    <t>ThingDef+Mech_RangedValkyrie.tools.left_fist.label</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.left_fist.label</t>
+  </si>
+  <si>
+    <t>left fist</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_RangedValkyrie.tools.right_fist.label</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.right_fist.label</t>
+  </si>
+  <si>
+    <t>right fist</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_RangedValkyrie.tools.head.label</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.head.label</t>
+  </si>
+  <si>
+    <t>head</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.description</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.description</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.label</t>
+  </si>
+  <si>
+    <t>melee valkyrie</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.left_fist.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.left_fist.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.right_fist.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.right_fist.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.head.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.head.label</t>
+  </si>
+  <si>
+    <t>PawnKindDef+Mech_MeleeValkyrie.label</t>
+  </si>
+  <si>
+    <t>PawnKindDef</t>
+  </si>
+  <si>
+    <t>PawnKindDef+Mech_RangedValkyrie.label</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger.label</t>
+  </si>
+  <si>
+    <t>stinger</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger.description</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger.description</t>
+  </si>
+  <si>
+    <t>A powerful mechanoid blade. Named for the wasp-like appearence of the mechanoids using it.</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger.tools.blade.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger.tools.blade.label</t>
+  </si>
+  <si>
+    <t>blade</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger.verbs.Verb_CooldownJump.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger.verbs.Verb_CooldownJump.label</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger_Leapless.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger_Leapless.label</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger_Leapless.description</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger_Leapless.description</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger_Leapless.tools.blade.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger_Leapless.tools.blade.label</t>
+  </si>
+  <si>
+    <t>ThingDef+PawnJumper_ValkyrieFlight.label</t>
+  </si>
+  <si>
+    <t>PawnJumper_ValkyrieFlight.label</t>
+  </si>
+  <si>
+    <t>flying</t>
+  </si>
+  <si>
+    <t>ThingDef+Gun_ValkyrieChargeSpear.label</t>
+  </si>
+  <si>
+    <t>Gun_ValkyrieChargeSpear.label</t>
+  </si>
+  <si>
+    <t>charge spear</t>
+  </si>
+  <si>
+    <t>ThingDef+Gun_ValkyrieChargeSpear.description</t>
+  </si>
+  <si>
+    <t>Gun_ValkyrieChargeSpear.description</t>
+  </si>
+  <si>
+    <t>A long-range weapon used by mechanoids. Fires three powerful charged projectiles in a short burst.</t>
+  </si>
+  <si>
+    <t>ThingDef+Gun_ValkyrieChargeSpear.verbs.Verb_Shoot.label</t>
+  </si>
+  <si>
+    <t>Gun_ValkyrieChargeSpear.verbs.Verb_Shoot.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Gun_ValkyrieChargeSpear.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>Gun_ValkyrieChargeSpear.tools.barrel.label</t>
+  </si>
+  <si>
+    <t>barrel</t>
+  </si>
+  <si>
+    <t>RecipeDef+Ranged_Valkyrie.jobString</t>
+  </si>
+  <si>
+    <t>RecipeDef</t>
+  </si>
+  <si>
+    <t>Ranged_Valkyrie.jobString</t>
+  </si>
+  <si>
+    <t>Biotech</t>
+  </si>
+  <si>
+    <t>Gestating mech.</t>
+  </si>
+  <si>
+    <t>RecipeDef+Ranged_Valkyrie.label</t>
+  </si>
+  <si>
+    <t>Ranged_Valkyrie.label</t>
+  </si>
+  <si>
+    <t>gestate ranged valkyrie</t>
+  </si>
+  <si>
+    <t>RecipeDef+Ranged_Valkyrie.description</t>
+  </si>
+  <si>
+    <t>Ranged_Valkyrie.description</t>
+  </si>
+  <si>
+    <t>Gestate a ranged valkyrie mechanoid.</t>
+  </si>
+  <si>
+    <t>RecipeDef+Melee_Valkyrie.jobString</t>
+  </si>
+  <si>
+    <t>Melee_Valkyrie.jobString</t>
+  </si>
+  <si>
+    <t>RecipeDef+Melee_Valkyrie.label</t>
+  </si>
+  <si>
+    <t>Melee_Valkyrie.label</t>
+  </si>
+  <si>
+    <t>gestate melee valkyrie</t>
+  </si>
+  <si>
+    <t>RecipeDef+Melee_Valkyrie.description</t>
+  </si>
+  <si>
+    <t>Melee_Valkyrie.description</t>
+  </si>
+  <si>
+    <t>워리어 발키리 메카노이드를 배양합니다.</t>
+  </si>
+  <si>
+    <t>워리어 발키리 배양</t>
+  </si>
+  <si>
+    <t>레인저 발키리 메카노이드를 배양합니다.</t>
+  </si>
+  <si>
+    <t>레인저 발키리 배양</t>
+  </si>
+  <si>
+    <t>총열</t>
+  </si>
+  <si>
+    <t>Gun_ValkyrieChargeSpear.tools.0.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Gun_ValkyrieChargeSpear.tools.0.label</t>
+  </si>
+  <si>
+    <t>칼날</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger_Leapless.tools.0.label</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger_Leapless.tools.0.label</t>
+  </si>
+  <si>
+    <t>MeleeValkyrieStinger.tools.0.label</t>
+  </si>
+  <si>
+    <t>ThingDef+MeleeValkyrieStinger.tools.0.label</t>
+  </si>
+  <si>
+    <t>레인저 발키리</t>
+  </si>
+  <si>
+    <t>워리어 발키리</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.2.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.2.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.1.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.1.label</t>
+  </si>
+  <si>
+    <t>Mech_MeleeValkyrie.tools.0.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_MeleeValkyrie.tools.0.label</t>
+  </si>
+  <si>
+    <t>날개가 달려 매우 빠르게 움직이는 메카노이드입니다. 내부 동력원에 충전이 필요하여 비행은 한 번에 1분 정도만 가능합니다. 일부 발키리는 날개 대신 다른 무기에 의존합니다.</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.2.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_RangedValkyrie.tools.2.label</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.1.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Mech_RangedValkyrie.tools.1.label</t>
+  </si>
+  <si>
+    <t>Mech_RangedValkyrie.tools.0.label</t>
+  </si>
+  <si>
     <t>ThingDef+Mech_RangedValkyrie.tools.0.label</t>
   </si>
   <si>
-    <t>Mech_RangedValkyrie.tools.0.label</t>
-  </si>
-  <si>
-    <t>left fist</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_RangedValkyrie.tools.1.label</t>
-  </si>
-  <si>
-    <t>Mech_RangedValkyrie.tools.1.label</t>
-  </si>
-  <si>
-    <t>right fist</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_RangedValkyrie.tools.2.label</t>
-  </si>
-  <si>
-    <t>Mech_RangedValkyrie.tools.2.label</t>
-  </si>
-  <si>
-    <t>head</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_MeleeValkyrie.description</t>
-  </si>
-  <si>
-    <t>Mech_MeleeValkyrie.description</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_MeleeValkyrie.label</t>
-  </si>
-  <si>
-    <t>Mech_MeleeValkyrie.label</t>
-  </si>
-  <si>
-    <t>melee valkyrie</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_MeleeValkyrie.tools.0.label</t>
-  </si>
-  <si>
-    <t>Mech_MeleeValkyrie.tools.0.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_MeleeValkyrie.tools.1.label</t>
-  </si>
-  <si>
-    <t>Mech_MeleeValkyrie.tools.1.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Mech_MeleeValkyrie.tools.2.label</t>
-  </si>
-  <si>
-    <t>Mech_MeleeValkyrie.tools.2.label</t>
-  </si>
-  <si>
-    <t>PawnKindDef+Mech_MeleeValkyrie.label</t>
-  </si>
-  <si>
-    <t>PawnKindDef</t>
-  </si>
-  <si>
-    <t>PawnKindDef+Mech_RangedValkyrie.label</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger.label</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger.label</t>
-  </si>
-  <si>
-    <t>stinger</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger.description</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger.description</t>
-  </si>
-  <si>
-    <t>A powerful mechanoid blade. Named for the wasp-like appearence of the mechanoids using it.</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger.tools.0.label</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger.tools.0.label</t>
-  </si>
-  <si>
-    <t>blade</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger.verbs.Verb_CooldownJump.label</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger.verbs.Verb_CooldownJump.label</t>
-  </si>
-  <si>
-    <t>jump</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger_Leapless.label</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger_Leapless.label</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger_Leapless.description</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger_Leapless.description</t>
-  </si>
-  <si>
-    <t>ThingDef+MeleeValkyrieStinger_Leapless.tools.0.label</t>
-  </si>
-  <si>
-    <t>MeleeValkyrieStinger_Leapless.tools.0.label</t>
-  </si>
-  <si>
-    <t>ThingDef+PawnJumper_ValkyrieFlight.label</t>
-  </si>
-  <si>
-    <t>PawnJumper_ValkyrieFlight.label</t>
-  </si>
-  <si>
-    <t>flying</t>
-  </si>
-  <si>
-    <t>ThingDef+Gun_ValkyrieChargeSpear.label</t>
-  </si>
-  <si>
-    <t>Gun_ValkyrieChargeSpear.label</t>
-  </si>
-  <si>
-    <t>charge spear</t>
-  </si>
-  <si>
-    <t>ThingDef+Gun_ValkyrieChargeSpear.description</t>
-  </si>
-  <si>
-    <t>Gun_ValkyrieChargeSpear.description</t>
-  </si>
-  <si>
-    <t>A long-range weapon used by mechanoids. Fires three powerful charged projectiles in a short burst.</t>
-  </si>
-  <si>
-    <t>ThingDef+Gun_ValkyrieChargeSpear.verbs.Verb_Shoot.label</t>
-  </si>
-  <si>
-    <t>Gun_ValkyrieChargeSpear.verbs.Verb_Shoot.label</t>
-  </si>
-  <si>
-    <t>ThingDef+Gun_ValkyrieChargeSpear.tools.0.label</t>
-  </si>
-  <si>
-    <t>Gun_ValkyrieChargeSpear.tools.0.label</t>
-  </si>
-  <si>
-    <t>barrel</t>
-  </si>
-  <si>
-    <t>RecipeDef+Ranged_Valkyrie.jobString</t>
-  </si>
-  <si>
-    <t>RecipeDef</t>
-  </si>
-  <si>
-    <t>Ranged_Valkyrie.jobString</t>
-  </si>
-  <si>
-    <t>Biotech</t>
-  </si>
-  <si>
-    <t>Gestating mech.</t>
-  </si>
-  <si>
-    <t>RecipeDef+Ranged_Valkyrie.label</t>
-  </si>
-  <si>
-    <t>Ranged_Valkyrie.label</t>
-  </si>
-  <si>
-    <t>gestate ranged valkyrie</t>
-  </si>
-  <si>
-    <t>RecipeDef+Ranged_Valkyrie.description</t>
-  </si>
-  <si>
-    <t>Ranged_Valkyrie.description</t>
-  </si>
-  <si>
-    <t>Gestate a ranged valkyrie mechanoid.</t>
-  </si>
-  <si>
-    <t>RecipeDef+Melee_Valkyrie.jobString</t>
-  </si>
-  <si>
-    <t>Melee_Valkyrie.jobString</t>
-  </si>
-  <si>
-    <t>RecipeDef+Melee_Valkyrie.label</t>
-  </si>
-  <si>
-    <t>Melee_Valkyrie.label</t>
-  </si>
-  <si>
-    <t>gestate melee valkyrie</t>
-  </si>
-  <si>
-    <t>RecipeDef+Melee_Valkyrie.description</t>
-  </si>
-  <si>
-    <t>Melee_Valkyrie.description</t>
-  </si>
-  <si>
-    <t>총열</t>
+    <t>밀리 발키리 메카노이드를 배양합니다.</t>
+  </si>
+  <si>
+    <t>밀리 발키리 배양</t>
+  </si>
+  <si>
+    <t>메카노이드 배양 중</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>레인지드 발키리 메카노이드를 배양합니다.</t>
+  </si>
+  <si>
+    <t>레인지드 발키리 배양</t>
   </si>
   <si>
     <t>차지 스피어</t>
@@ -302,6 +398,9 @@
     <t>메카노이드가 사용하는 장거리 무기입니다. 세 개의 강력한 전자기 탄환을 한 번에 발사합니다.</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>칼날</t>
   </si>
   <si>
@@ -314,6 +413,12 @@
     <t>비행</t>
   </si>
   <si>
+    <t>레인지드 발키리</t>
+  </si>
+  <si>
+    <t>밀리 발키리</t>
+  </si>
+  <si>
     <t>머리</t>
   </si>
   <si>
@@ -323,31 +428,25 @@
     <t>왼쪽 주먹</t>
   </si>
   <si>
-    <t>밀리 발키리</t>
-  </si>
-  <si>
     <t>날개가 달린 매우 민첩한 메카노이드입니다. 무한한 동력원을 가졌음에도 불구하고 비행에는 내부 커패시터에 의한 일시적인 전력 증폭이 필요합니다. 충전에 걸리는 시간 때문에 비행 후 다시 비행하려면 수 분 정도를 기다려야 합니다. 일부 발키리는 날개가 없는 대신 다른 무기에 의존합니다.</t>
   </si>
   <si>
-    <t>레인지드 발키리</t>
-  </si>
-  <si>
-    <t>밀리 발키리 메카노이드를 배양합니다.</t>
-  </si>
-  <si>
-    <t>밀리 발키리 배양</t>
-  </si>
-  <si>
-    <t>레인지드 발키리 메카노이드를 배양합니다.</t>
-  </si>
-  <si>
-    <t>레인지드 발키리 배양</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>메카노이드 배양 중</t>
+    <t>강력한 메카노이드 칼날입니다. 이것을 사용하는 메카노이드의 모습이 말벌과 닮아 붙여진 이름입니다.</t>
+  </si>
+  <si>
+    <t>손잡이</t>
+  </si>
+  <si>
+    <t>메카노이드가 사용하는 원거리 무기입니다. 한번에 강력한 에너지 포탄 3발을 발사합니다.</t>
+  </si>
+  <si>
+    <t>왼주먹</t>
+  </si>
+  <si>
+    <t>오른주먹</t>
+  </si>
+  <si>
+    <t>비행 중</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -355,7 +454,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -371,6 +470,12 @@
     <font>
       <sz val="8"/>
       <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="돋움체"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -703,7 +808,580 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="63.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4575F10-A8D5-4896-A2A3-73F9952FE219}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -751,7 +1429,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -768,58 +1446,58 @@
         <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -836,7 +1514,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -853,58 +1531,58 @@
         <v>26</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -921,7 +1599,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -938,7 +1616,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -955,7 +1633,7 @@
         <v>38</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -972,24 +1650,24 @@
         <v>41</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
@@ -1006,7 +1684,7 @@
         <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -1023,7 +1701,7 @@
         <v>38</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
@@ -1040,24 +1718,24 @@
         <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
@@ -1074,7 +1752,7 @@
         <v>56</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -1091,7 +1769,7 @@
         <v>59</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1108,7 +1786,7 @@
         <v>62</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -1125,24 +1803,24 @@
         <v>59</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -1162,7 +1840,7 @@
         <v>72</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
@@ -1182,7 +1860,7 @@
         <v>75</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -1202,7 +1880,7 @@
         <v>78</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
@@ -1222,7 +1900,7 @@
         <v>72</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -1242,7 +1920,7 @@
         <v>83</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -1262,7 +1940,7 @@
         <v>78</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>